<commit_message>
Added experiment3 notebook for external tests
</commit_message>
<xml_diff>
--- a/src/Gabriel/Deliverable/Evaluation.xlsx
+++ b/src/Gabriel/Deliverable/Evaluation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="292">
   <si>
     <t>Algorithm</t>
   </si>
@@ -838,13 +838,67 @@
   </si>
   <si>
     <t>FMeasure: 54.5689569156%</t>
+  </si>
+  <si>
+    <t>Accuracy: 68.1133212779%</t>
+  </si>
+  <si>
+    <t>Precision: 73.2057779175%</t>
+  </si>
+  <si>
+    <t>Recall: 68.1133212779%</t>
+  </si>
+  <si>
+    <t>FMeasure: 69.921196765%</t>
+  </si>
+  <si>
+    <t>Accuracy: 69.7%</t>
+  </si>
+  <si>
+    <t>Precision: 69.9594432532%</t>
+  </si>
+  <si>
+    <t>Recall: 69.7%</t>
+  </si>
+  <si>
+    <t>FMeasure: 68.5782038492%</t>
+  </si>
+  <si>
+    <t>max_depth=2</t>
+  </si>
+  <si>
+    <t>random_state=500</t>
+  </si>
+  <si>
+    <t>Accuracy: 69.85%</t>
+  </si>
+  <si>
+    <t>Precision: 70.0042833175%</t>
+  </si>
+  <si>
+    <t>Recall: 69.85%</t>
+  </si>
+  <si>
+    <t>FMeasure: 68.8519520799%</t>
+  </si>
+  <si>
+    <t>Accuracy: 70.323488045%</t>
+  </si>
+  <si>
+    <t>Precision: 73.3411852562%</t>
+  </si>
+  <si>
+    <t>Recall: 70.323488045%</t>
+  </si>
+  <si>
+    <t>FMeasure: 71.5289315994%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -879,6 +933,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -900,7 +960,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -911,6 +971,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,6 +983,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -968,7 +1034,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1003,7 +1069,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1212,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J132"/>
+  <dimension ref="A1:J143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E100" workbookViewId="0">
-      <selection activeCell="G116" sqref="G116"/>
+    <sheetView tabSelected="1" topLeftCell="E121" workbookViewId="0">
+      <selection activeCell="H129" sqref="H129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3265,6 +3331,145 @@
       </c>
       <c r="I132" s="2" t="s">
         <v>273</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F133" s="3">
+        <v>0</v>
+      </c>
+      <c r="G133" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H133" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="I133" s="6" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B134" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H134" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="I134" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B135" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H135" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I135" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B136" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H136" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="I136" s="6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B137" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F138" s="3">
+        <v>0</v>
+      </c>
+      <c r="G138" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H138" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="I138" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B139" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H139" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="I139" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B140" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H140" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="I140" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B141" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H141" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="I141" s="6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B142" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B143" s="3" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>